<commit_message>
Lots of minor refactoring
</commit_message>
<xml_diff>
--- a/livelib/tests/data/sample/test_export/xlsx/create_file/Eugenia_Novik-correct_output.xlsx
+++ b/livelib/tests/data/sample/test_export/xlsx/create_file/Eugenia_Novik-correct_output.xlsx
@@ -26,12 +26,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <name val="Cambria"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <b val="1"/>
       <color theme="3"/>
-      <sz val="18"/>
-      <scheme val="major"/>
+      <sz val="13"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <name val="Calibri"/>
@@ -49,7 +49,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -57,15 +57,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.5"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
@@ -79,7 +88,7 @@
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
-    <cellStyle name="Title" xfId="1" builtinId="15" hidden="0"/>
+    <cellStyle name="Headline 2" xfId="1" builtinId="17" hidden="0"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>

</xml_diff>

<commit_message>
Bug with db in test_export
</commit_message>
<xml_diff>
--- a/livelib/tests/data/sample/test_export/xlsx/create_file/Eugenia_Novik-correct_output.xlsx
+++ b/livelib/tests/data/sample/test_export/xlsx/create_file/Eugenia_Novik-correct_output.xlsx
@@ -569,7 +569,7 @@
       </c>
       <c r="I2" s="2" t="inlineStr"/>
       <c r="J2" t="n">
-        <v>4.12</v>
+        <v>4.11</v>
       </c>
       <c r="K2" s="2" t="inlineStr"/>
       <c r="L2" s="2" t="inlineStr">
@@ -1073,7 +1073,7 @@
       </c>
       <c r="I14" s="2" t="inlineStr"/>
       <c r="J14" t="n">
-        <v>4.6</v>
+        <v>4.58</v>
       </c>
       <c r="K14" s="2" t="inlineStr"/>
       <c r="L14" s="2" t="inlineStr">
@@ -1199,7 +1199,7 @@
       </c>
       <c r="I17" s="2" t="inlineStr"/>
       <c r="J17" t="n">
-        <v>4.48</v>
+        <v>4.46</v>
       </c>
       <c r="K17" s="2" t="inlineStr"/>
       <c r="L17" s="2" t="inlineStr">
@@ -1577,7 +1577,7 @@
       </c>
       <c r="I26" s="2" t="inlineStr"/>
       <c r="J26" t="n">
-        <v>3.58</v>
+        <v>3.63</v>
       </c>
       <c r="K26" s="2" t="inlineStr"/>
       <c r="L26" s="2" t="inlineStr">
@@ -1661,7 +1661,7 @@
       </c>
       <c r="I28" s="2" t="inlineStr"/>
       <c r="J28" t="n">
-        <v>4.08</v>
+        <v>4.07</v>
       </c>
       <c r="K28" s="2" t="inlineStr"/>
       <c r="L28" s="2" t="inlineStr">
@@ -1997,7 +1997,7 @@
       </c>
       <c r="I36" s="2" t="inlineStr"/>
       <c r="J36" t="n">
-        <v>4.7</v>
+        <v>4.8</v>
       </c>
       <c r="K36" s="2" t="inlineStr"/>
       <c r="L36" s="2" t="inlineStr">
@@ -2039,7 +2039,7 @@
       </c>
       <c r="I37" s="2" t="inlineStr"/>
       <c r="J37" t="n">
-        <v>3.67</v>
+        <v>3.64</v>
       </c>
       <c r="K37" s="2" t="inlineStr"/>
       <c r="L37" s="2" t="inlineStr">
@@ -2081,7 +2081,7 @@
       </c>
       <c r="I38" s="2" t="inlineStr"/>
       <c r="J38" t="n">
-        <v>4.33</v>
+        <v>4.31</v>
       </c>
       <c r="K38" s="2" t="inlineStr"/>
       <c r="L38" s="2" t="inlineStr">
@@ -2291,7 +2291,7 @@
       </c>
       <c r="I43" s="2" t="inlineStr"/>
       <c r="J43" t="n">
-        <v>3.82</v>
+        <v>3.81</v>
       </c>
       <c r="K43" s="2" t="inlineStr"/>
       <c r="L43" s="2" t="inlineStr">
@@ -2459,7 +2459,7 @@
       </c>
       <c r="I47" s="2" t="inlineStr"/>
       <c r="J47" t="n">
-        <v>3</v>
+        <v>3.02</v>
       </c>
       <c r="K47" s="2" t="inlineStr"/>
       <c r="L47" s="2" t="inlineStr">
@@ -2501,7 +2501,7 @@
       </c>
       <c r="I48" s="2" t="inlineStr"/>
       <c r="J48" t="n">
-        <v>4.16</v>
+        <v>4.17</v>
       </c>
       <c r="K48" s="2" t="inlineStr"/>
       <c r="L48" s="2" t="inlineStr">
@@ -2513,16 +2513,16 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Prince's Gambit</t>
+          <t>Дни нашей жизни</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>C. S. Pacat</t>
+          <t>Микита Франко</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D49" t="inlineStr"/>
       <c r="E49" t="inlineStr"/>
@@ -2533,34 +2533,34 @@
       </c>
       <c r="G49" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/author/727234</t>
+          <t>https://livelib.ru/author/1332952</t>
         </is>
       </c>
       <c r="H49" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/book/1001527382</t>
+          <t>https://livelib.ru/book/1003973497</t>
         </is>
       </c>
       <c r="I49" s="2" t="inlineStr"/>
       <c r="J49" t="n">
-        <v>4.45</v>
+        <v>4.4</v>
       </c>
       <c r="K49" s="2" t="inlineStr"/>
       <c r="L49" s="2" t="inlineStr">
         <is>
-          <t>https://s1.livelib.ru/boocover/1001527382/70/36c6/C._S._Pacat__Princes_Gambit.jpg</t>
+          <t>https://s1.livelib.ru/boocover/1003973497/70/0a3d/Mikita_Franko__Dni_nashej_zhizni.jpg</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Memo. Секреты создания структуры и персонажей в сценарии</t>
+          <t>Prince's Gambit</t>
         </is>
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>Кристофер Воглер</t>
+          <t>C. S. Pacat</t>
         </is>
       </c>
       <c r="C50" t="n">
@@ -2570,43 +2570,43 @@
       <c r="E50" t="inlineStr"/>
       <c r="F50" t="inlineStr">
         <is>
-          <t>2022 ноябрь</t>
+          <t>2022 декабрь</t>
         </is>
       </c>
       <c r="G50" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/author/599800</t>
+          <t>https://livelib.ru/author/727234</t>
         </is>
       </c>
       <c r="H50" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/book/1002783998</t>
+          <t>https://livelib.ru/book/1001527382</t>
         </is>
       </c>
       <c r="I50" s="2" t="inlineStr"/>
       <c r="J50" t="n">
-        <v>4.23</v>
+        <v>4.44</v>
       </c>
       <c r="K50" s="2" t="inlineStr"/>
       <c r="L50" s="2" t="inlineStr">
         <is>
-          <t>https://s1.livelib.ru/boocover/1002783998/70/0bf4/__Memo._Sekrety_sozdaniya_struktury_i_personazhej_v_stsenarii.jpg</t>
+          <t>https://s1.livelib.ru/boocover/1001527382/70/36c6/C._S._Pacat__Princes_Gambit.jpg</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Плененный принц</t>
+          <t>Memo. Секреты создания структуры и персонажей в сценарии</t>
         </is>
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>К. С. Пакат</t>
+          <t>Кристофер Воглер</t>
         </is>
       </c>
       <c r="C51" t="n">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="D51" t="inlineStr"/>
       <c r="E51" t="inlineStr"/>
@@ -2617,34 +2617,34 @@
       </c>
       <c r="G51" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/author/727234</t>
+          <t>https://livelib.ru/author/599800</t>
         </is>
       </c>
       <c r="H51" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/book/1006860844</t>
+          <t>https://livelib.ru/book/1002783998</t>
         </is>
       </c>
       <c r="I51" s="2" t="inlineStr"/>
       <c r="J51" t="n">
-        <v>3.8</v>
+        <v>4.25</v>
       </c>
       <c r="K51" s="2" t="inlineStr"/>
       <c r="L51" s="2" t="inlineStr">
         <is>
-          <t>https://s1.livelib.ru/boocover/1006860844/70/545f/K._S._Pakat__Plenennyj_prints.jpg</t>
+          <t>https://s1.livelib.ru/boocover/1002783998/70/0bf4/__Memo._Sekrety_sozdaniya_struktury_i_personazhej_v_stsenarii.jpg</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>A Simple Heart</t>
+          <t>Плененный принц</t>
         </is>
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>Gustave Flaubert</t>
+          <t>К. С. Пакат</t>
         </is>
       </c>
       <c r="C52" t="n">
@@ -2659,34 +2659,34 @@
       </c>
       <c r="G52" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/author/322</t>
+          <t>https://livelib.ru/author/727234</t>
         </is>
       </c>
       <c r="H52" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/book/1001646231</t>
+          <t>https://livelib.ru/book/1006860844</t>
         </is>
       </c>
       <c r="I52" s="2" t="inlineStr"/>
       <c r="J52" t="n">
-        <v>3.77</v>
+        <v>3.8</v>
       </c>
       <c r="K52" s="2" t="inlineStr"/>
       <c r="L52" s="2" t="inlineStr">
         <is>
-          <t>https://s1.livelib.ru/boocover/1001646231/70/b70f/Gustave_Flaubert__A_Simple_Heart.jpg</t>
+          <t>https://s1.livelib.ru/boocover/1006860844/70/545f/K._S._Pakat__Plenennyj_prints.jpg</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Краткая история пьянства от каменного века до наших дней. Что, где, когда и по какому поводу</t>
+          <t>A Simple Heart</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Марк Форсайт</t>
+          <t>Gustave Flaubert</t>
         </is>
       </c>
       <c r="C53" t="n">
@@ -2701,38 +2701,38 @@
       </c>
       <c r="G53" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/author/1103781</t>
+          <t>https://livelib.ru/author/322</t>
         </is>
       </c>
       <c r="H53" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/book/1002809862</t>
+          <t>https://livelib.ru/book/1001646231</t>
         </is>
       </c>
       <c r="I53" s="2" t="inlineStr"/>
       <c r="J53" t="n">
-        <v>3.87</v>
+        <v>3.75</v>
       </c>
       <c r="K53" s="2" t="inlineStr"/>
       <c r="L53" s="2" t="inlineStr">
         <is>
-          <t>https://s1.livelib.ru/boocover/1002809862/70/6ca8/Mark_Forsajt__Kratkaya_istoriya_pyanstva_ot_kamennogo_veka_do_nashih_dnej._Chto_.jpg</t>
+          <t>https://s1.livelib.ru/boocover/1001646231/70/b70f/Gustave_Flaubert__A_Simple_Heart.jpg</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Без ума от Венсана</t>
+          <t>Краткая история пьянства от каменного века до наших дней. Что, где, когда и по какому поводу</t>
         </is>
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Эрве Гибер</t>
+          <t>Марк Форсайт</t>
         </is>
       </c>
       <c r="C54" t="n">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="D54" t="inlineStr"/>
       <c r="E54" t="inlineStr"/>
@@ -2743,38 +2743,38 @@
       </c>
       <c r="G54" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/author/234378</t>
+          <t>https://livelib.ru/author/1103781</t>
         </is>
       </c>
       <c r="H54" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/book/1000538931</t>
+          <t>https://livelib.ru/book/1002809862</t>
         </is>
       </c>
       <c r="I54" s="2" t="inlineStr"/>
       <c r="J54" t="n">
-        <v>3.77</v>
+        <v>3.87</v>
       </c>
       <c r="K54" s="2" t="inlineStr"/>
       <c r="L54" s="2" t="inlineStr">
         <is>
-          <t>https://s1.livelib.ru/boocover/1000538931/70/2256/Erve_Giber__Bez_uma_ot_Vensana.jpg</t>
+          <t>https://s1.livelib.ru/boocover/1002809862/70/6ca8/Mark_Forsajt__Kratkaya_istoriya_pyanstva_ot_kamennogo_veka_do_nashih_dnej._Chto_.jpg</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Воскрешение</t>
+          <t>Без ума от Венсана</t>
         </is>
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>Брайан Кин</t>
+          <t>Эрве Гибер</t>
         </is>
       </c>
       <c r="C55" t="n">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="D55" t="inlineStr"/>
       <c r="E55" t="inlineStr"/>
@@ -2785,38 +2785,38 @@
       </c>
       <c r="G55" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/author/513369</t>
+          <t>https://livelib.ru/author/234378</t>
         </is>
       </c>
       <c r="H55" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/book/1004575657</t>
+          <t>https://livelib.ru/book/1000538931</t>
         </is>
       </c>
       <c r="I55" s="2" t="inlineStr"/>
       <c r="J55" t="n">
-        <v>3.65</v>
+        <v>3.77</v>
       </c>
       <c r="K55" s="2" t="inlineStr"/>
       <c r="L55" s="2" t="inlineStr">
         <is>
-          <t>https://s1.livelib.ru/boocover/1004575657/70/0455/Brajan_Kin__Voskreshenie.jpg</t>
+          <t>https://s1.livelib.ru/boocover/1000538931/70/2256/Erve_Giber__Bez_uma_ot_Vensana.jpg</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Крабы-убийцы</t>
+          <t>Воскрешение</t>
         </is>
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>Гай Н. Смит</t>
+          <t>Брайан Кин</t>
         </is>
       </c>
       <c r="C56" t="n">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="D56" t="inlineStr"/>
       <c r="E56" t="inlineStr"/>
@@ -2827,38 +2827,38 @@
       </c>
       <c r="G56" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/author/236842</t>
+          <t>https://livelib.ru/author/513369</t>
         </is>
       </c>
       <c r="H56" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/book/1004575648</t>
+          <t>https://livelib.ru/book/1004575657</t>
         </is>
       </c>
       <c r="I56" s="2" t="inlineStr"/>
       <c r="J56" t="n">
-        <v>2.9</v>
+        <v>3.65</v>
       </c>
       <c r="K56" s="2" t="inlineStr"/>
       <c r="L56" s="2" t="inlineStr">
         <is>
-          <t>https://s1.livelib.ru/boocover/1004575648/70/f03b/Gaj_N._Smit__Krabyubijtsy.jpg</t>
+          <t>https://s1.livelib.ru/boocover/1004575657/70/0455/Brajan_Kin__Voskreshenie.jpg</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>Песнь Кали</t>
+          <t>Крабы-убийцы</t>
         </is>
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>Дэн Симмонс</t>
+          <t>Гай Н. Смит</t>
         </is>
       </c>
       <c r="C57" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D57" t="inlineStr"/>
       <c r="E57" t="inlineStr"/>
@@ -2869,38 +2869,38 @@
       </c>
       <c r="G57" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/author/679</t>
+          <t>https://livelib.ru/author/236842</t>
         </is>
       </c>
       <c r="H57" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/book/1000546271</t>
+          <t>https://livelib.ru/book/1004575648</t>
         </is>
       </c>
       <c r="I57" s="2" t="inlineStr"/>
       <c r="J57" t="n">
-        <v>3.77</v>
+        <v>2.9</v>
       </c>
       <c r="K57" s="2" t="inlineStr"/>
       <c r="L57" s="2" t="inlineStr">
         <is>
-          <t>https://s1.livelib.ru/boocover/1000546271/70/9498/Den_Simmons__Pesn_Kali.jpg</t>
+          <t>https://s1.livelib.ru/boocover/1004575648/70/f03b/Gaj_N._Smit__Krabyubijtsy.jpg</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>Succulent Prey</t>
+          <t>Песнь Кали</t>
         </is>
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>Wrath James White</t>
+          <t>Дэн Симмонс</t>
         </is>
       </c>
       <c r="C58" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D58" t="inlineStr"/>
       <c r="E58" t="inlineStr"/>
@@ -2911,38 +2911,38 @@
       </c>
       <c r="G58" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/author/642032</t>
+          <t>https://livelib.ru/author/679</t>
         </is>
       </c>
       <c r="H58" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/book/1003577361</t>
+          <t>https://livelib.ru/book/1000546271</t>
         </is>
       </c>
       <c r="I58" s="2" t="inlineStr"/>
       <c r="J58" t="n">
-        <v>3.38</v>
+        <v>3.76</v>
       </c>
       <c r="K58" s="2" t="inlineStr"/>
       <c r="L58" s="2" t="inlineStr">
         <is>
-          <t>https://s1.livelib.ru/boocover/1003577361/70/ac29/Wrath_James_White__Succulent_Prey.jpg</t>
+          <t>https://s1.livelib.ru/boocover/1000546271/70/9498/Den_Simmons__Pesn_Kali.jpg</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>Посылка</t>
+          <t>Succulent Prey</t>
         </is>
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>Себастьян Фитцек</t>
+          <t>Wrath James White</t>
         </is>
       </c>
       <c r="C59" t="n">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="D59" t="inlineStr"/>
       <c r="E59" t="inlineStr"/>
@@ -2953,64 +2953,64 @@
       </c>
       <c r="G59" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/author/230060</t>
+          <t>https://livelib.ru/author/642032</t>
         </is>
       </c>
       <c r="H59" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/book/1002704443</t>
+          <t>https://livelib.ru/book/1003577361</t>
         </is>
       </c>
       <c r="I59" s="2" t="inlineStr"/>
       <c r="J59" t="n">
-        <v>3.83</v>
+        <v>3.38</v>
       </c>
       <c r="K59" s="2" t="inlineStr"/>
       <c r="L59" s="2" t="inlineStr">
         <is>
-          <t>https://s1.livelib.ru/boocover/1002704443/70/9b5e/Sebastyan_Fittsek__Posylka.jpg</t>
+          <t>https://s1.livelib.ru/boocover/1003577361/70/ac29/Wrath_James_White__Succulent_Prey.jpg</t>
         </is>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>Дни нашей жизни</t>
+          <t>Посылка</t>
         </is>
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>Микита Франко</t>
+          <t>Себастьян Фитцек</t>
         </is>
       </c>
       <c r="C60" t="n">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="D60" t="inlineStr"/>
       <c r="E60" t="inlineStr"/>
       <c r="F60" t="inlineStr">
         <is>
-          <t>2022 декабрь</t>
+          <t>2022 ноябрь</t>
         </is>
       </c>
       <c r="G60" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/author/1332952</t>
+          <t>https://livelib.ru/author/230060</t>
         </is>
       </c>
       <c r="H60" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/book/1003973497</t>
+          <t>https://livelib.ru/book/1002704443</t>
         </is>
       </c>
       <c r="I60" s="2" t="inlineStr"/>
       <c r="J60" t="n">
-        <v>4.4</v>
+        <v>3.84</v>
       </c>
       <c r="K60" s="2" t="inlineStr"/>
       <c r="L60" s="2" t="inlineStr">
         <is>
-          <t>https://s1.livelib.ru/boocover/1003973497/70/0a3d/Mikita_Franko__Dni_nashej_zhizni.jpg</t>
+          <t>https://s1.livelib.ru/boocover/1002704443/70/9b5e/Sebastyan_Fittsek__Posylka.jpg</t>
         </is>
       </c>
     </row>
@@ -3047,7 +3047,7 @@
       </c>
       <c r="I61" s="2" t="inlineStr"/>
       <c r="J61" t="n">
-        <v>3.27</v>
+        <v>3.18</v>
       </c>
       <c r="K61" s="2" t="inlineStr"/>
       <c r="L61" s="2" t="inlineStr">
@@ -3341,7 +3341,7 @@
       </c>
       <c r="I68" s="2" t="inlineStr"/>
       <c r="J68" t="n">
-        <v>4.06</v>
+        <v>4.07</v>
       </c>
       <c r="K68" s="2" t="inlineStr"/>
       <c r="L68" s="2" t="inlineStr">
@@ -3467,7 +3467,7 @@
       </c>
       <c r="I71" s="2" t="inlineStr"/>
       <c r="J71" t="n">
-        <v>3.94</v>
+        <v>3.93</v>
       </c>
       <c r="K71" s="2" t="inlineStr"/>
       <c r="L71" s="2" t="inlineStr">
@@ -3543,7 +3543,7 @@
       </c>
       <c r="I73" s="2" t="inlineStr"/>
       <c r="J73" t="n">
-        <v>3.77</v>
+        <v>3.78</v>
       </c>
       <c r="K73" s="2" t="inlineStr"/>
       <c r="L73" s="2" t="inlineStr">
@@ -3585,7 +3585,7 @@
       </c>
       <c r="I74" s="2" t="inlineStr"/>
       <c r="J74" t="n">
-        <v>4.33</v>
+        <v>4.32</v>
       </c>
       <c r="K74" s="2" t="inlineStr"/>
       <c r="L74" s="2" t="inlineStr">
@@ -3669,7 +3669,7 @@
       </c>
       <c r="I76" s="2" t="inlineStr"/>
       <c r="J76" t="n">
-        <v>3.29</v>
+        <v>3.3</v>
       </c>
       <c r="K76" s="2" t="inlineStr"/>
       <c r="L76" s="2" t="inlineStr">
@@ -3711,7 +3711,7 @@
       </c>
       <c r="I77" s="2" t="inlineStr"/>
       <c r="J77" t="n">
-        <v>4.29</v>
+        <v>4.3</v>
       </c>
       <c r="K77" s="2" t="inlineStr"/>
       <c r="L77" s="2" t="inlineStr">
@@ -4383,7 +4383,7 @@
       </c>
       <c r="I93" s="2" t="inlineStr"/>
       <c r="J93" t="n">
-        <v>4.21</v>
+        <v>4.19</v>
       </c>
       <c r="K93" s="2" t="inlineStr"/>
       <c r="L93" s="2" t="inlineStr">
@@ -4593,7 +4593,7 @@
       </c>
       <c r="I98" s="2" t="inlineStr"/>
       <c r="J98" t="n">
-        <v>2.91</v>
+        <v>2.93</v>
       </c>
       <c r="K98" s="2" t="inlineStr"/>
       <c r="L98" s="2" t="inlineStr">
@@ -4803,7 +4803,7 @@
       </c>
       <c r="I103" s="2" t="inlineStr"/>
       <c r="J103" t="n">
-        <v>4.4</v>
+        <v>4.39</v>
       </c>
       <c r="K103" s="2" t="inlineStr"/>
       <c r="L103" s="2" t="inlineStr">
@@ -4845,7 +4845,7 @@
       </c>
       <c r="I104" s="2" t="inlineStr"/>
       <c r="J104" t="n">
-        <v>0</v>
+        <v>4.34</v>
       </c>
       <c r="K104" s="2" t="inlineStr"/>
       <c r="L104" s="2" t="inlineStr">
@@ -4887,7 +4887,7 @@
       </c>
       <c r="I105" s="2" t="inlineStr"/>
       <c r="J105" t="n">
-        <v>3.65</v>
+        <v>3.67</v>
       </c>
       <c r="K105" s="2" t="inlineStr"/>
       <c r="L105" s="2" t="inlineStr">
@@ -4971,7 +4971,7 @@
       </c>
       <c r="I107" s="2" t="inlineStr"/>
       <c r="J107" t="n">
-        <v>4.48</v>
+        <v>4.47</v>
       </c>
       <c r="K107" s="2" t="inlineStr"/>
       <c r="L107" s="2" t="inlineStr">
@@ -5895,7 +5895,7 @@
       </c>
       <c r="I129" s="2" t="inlineStr"/>
       <c r="J129" t="n">
-        <v>3.31</v>
+        <v>3.32</v>
       </c>
       <c r="K129" s="2" t="inlineStr"/>
       <c r="L129" s="2" t="inlineStr">
@@ -5937,7 +5937,7 @@
       </c>
       <c r="I130" s="2" t="inlineStr"/>
       <c r="J130" t="n">
-        <v>3.96</v>
+        <v>3.95</v>
       </c>
       <c r="K130" s="2" t="inlineStr"/>
       <c r="L130" s="2" t="inlineStr">
@@ -6147,7 +6147,7 @@
       </c>
       <c r="I135" s="2" t="inlineStr"/>
       <c r="J135" t="n">
-        <v>3.31</v>
+        <v>3.27</v>
       </c>
       <c r="K135" s="2" t="inlineStr"/>
       <c r="L135" s="2" t="inlineStr">
@@ -6441,7 +6441,7 @@
       </c>
       <c r="I142" s="2" t="inlineStr"/>
       <c r="J142" t="n">
-        <v>4.06</v>
+        <v>4.08</v>
       </c>
       <c r="K142" s="2" t="inlineStr"/>
       <c r="L142" s="2" t="inlineStr">
@@ -6567,7 +6567,7 @@
       </c>
       <c r="I145" s="2" t="inlineStr"/>
       <c r="J145" t="n">
-        <v>3.39</v>
+        <v>3.4</v>
       </c>
       <c r="K145" s="2" t="inlineStr"/>
       <c r="L145" s="2" t="inlineStr">
@@ -6609,7 +6609,7 @@
       </c>
       <c r="I146" s="2" t="inlineStr"/>
       <c r="J146" t="n">
-        <v>4.39</v>
+        <v>4.4</v>
       </c>
       <c r="K146" s="2" t="inlineStr"/>
       <c r="L146" s="2" t="inlineStr">
@@ -6945,7 +6945,7 @@
       </c>
       <c r="I154" s="2" t="inlineStr"/>
       <c r="J154" t="n">
-        <v>3.9</v>
+        <v>3.89</v>
       </c>
       <c r="K154" s="2" t="inlineStr"/>
       <c r="L154" s="2" t="inlineStr">
@@ -7029,7 +7029,7 @@
       </c>
       <c r="I156" s="2" t="inlineStr"/>
       <c r="J156" t="n">
-        <v>3.82</v>
+        <v>3.81</v>
       </c>
       <c r="K156" s="2" t="inlineStr"/>
       <c r="L156" s="2" t="inlineStr">
@@ -7323,7 +7323,7 @@
       </c>
       <c r="I163" s="2" t="inlineStr"/>
       <c r="J163" t="n">
-        <v>4.26</v>
+        <v>4.25</v>
       </c>
       <c r="K163" s="2" t="inlineStr"/>
       <c r="L163" s="2" t="inlineStr">
@@ -7533,7 +7533,7 @@
       </c>
       <c r="I168" s="2" t="inlineStr"/>
       <c r="J168" t="n">
-        <v>4.19</v>
+        <v>4.18</v>
       </c>
       <c r="K168" s="2" t="inlineStr"/>
       <c r="L168" s="2" t="inlineStr">
@@ -7827,7 +7827,7 @@
       </c>
       <c r="I175" s="2" t="inlineStr"/>
       <c r="J175" t="n">
-        <v>4.32</v>
+        <v>4.33</v>
       </c>
       <c r="K175" s="2" t="inlineStr"/>
       <c r="L175" s="2" t="inlineStr">
@@ -8331,7 +8331,7 @@
       </c>
       <c r="I187" s="2" t="inlineStr"/>
       <c r="J187" t="n">
-        <v>4.06</v>
+        <v>4.07</v>
       </c>
       <c r="K187" s="2" t="inlineStr"/>
       <c r="L187" s="2" t="inlineStr">
@@ -8373,7 +8373,7 @@
       </c>
       <c r="I188" s="2" t="inlineStr"/>
       <c r="J188" t="n">
-        <v>4.08</v>
+        <v>4.07</v>
       </c>
       <c r="K188" s="2" t="inlineStr"/>
       <c r="L188" s="2" t="inlineStr">
@@ -8751,7 +8751,7 @@
       </c>
       <c r="I197" s="2" t="inlineStr"/>
       <c r="J197" t="n">
-        <v>2.92</v>
+        <v>2.95</v>
       </c>
       <c r="K197" s="2" t="inlineStr"/>
       <c r="L197" s="2" t="inlineStr">
@@ -9129,7 +9129,7 @@
       </c>
       <c r="I206" s="2" t="inlineStr"/>
       <c r="J206" t="n">
-        <v>4.12</v>
+        <v>4.11</v>
       </c>
       <c r="K206" s="2" t="inlineStr"/>
       <c r="L206" s="2" t="inlineStr">
@@ -9213,7 +9213,7 @@
       </c>
       <c r="I208" s="2" t="inlineStr"/>
       <c r="J208" t="n">
-        <v>3.9</v>
+        <v>3.89</v>
       </c>
       <c r="K208" s="2" t="inlineStr"/>
       <c r="L208" s="2" t="inlineStr">
@@ -9225,16 +9225,16 @@
     <row r="209">
       <c r="A209" t="inlineStr">
         <is>
-          <t>Последний шанс</t>
+          <t>Бессонница</t>
         </is>
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Федерико Аксат</t>
+          <t>Стивен Кинг</t>
         </is>
       </c>
       <c r="C209" t="n">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="D209" t="inlineStr"/>
       <c r="E209" t="inlineStr"/>
@@ -9245,38 +9245,38 @@
       </c>
       <c r="G209" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/author/1068951</t>
+          <t>https://livelib.ru/author/48</t>
         </is>
       </c>
       <c r="H209" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/book/1002688107</t>
+          <t>https://livelib.ru/book/1000465112</t>
         </is>
       </c>
       <c r="I209" s="2" t="inlineStr"/>
       <c r="J209" t="n">
-        <v>4.06</v>
+        <v>3.97</v>
       </c>
       <c r="K209" s="2" t="inlineStr"/>
       <c r="L209" s="2" t="inlineStr">
         <is>
-          <t>https://s1.livelib.ru/boocover/1002688107/70/e2c6/Federiko_Aksat__Poslednij_shans.jpg</t>
+          <t>https://s1.livelib.ru/boocover/1000465112/70/5b0b/Stiven_King__Bessonnitsa.jpg</t>
         </is>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
         <is>
-          <t>Wizard and Glass</t>
+          <t>Последний шанс</t>
         </is>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>Stephen King</t>
+          <t>Федерико Аксат</t>
         </is>
       </c>
       <c r="C210" t="n">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="D210" t="inlineStr"/>
       <c r="E210" t="inlineStr"/>
@@ -9287,80 +9287,80 @@
       </c>
       <c r="G210" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/author/48</t>
+          <t>https://livelib.ru/author/1068951</t>
         </is>
       </c>
       <c r="H210" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/book/1001001100</t>
+          <t>https://livelib.ru/book/1002688107</t>
         </is>
       </c>
       <c r="I210" s="2" t="inlineStr"/>
       <c r="J210" t="n">
-        <v>4.47</v>
+        <v>4.06</v>
       </c>
       <c r="K210" s="2" t="inlineStr"/>
       <c r="L210" s="2" t="inlineStr">
         <is>
-          <t>https://s1.livelib.ru/boocover/1001001100/70/dc68/Stephen_King__Wizard_and_Glass.jpg</t>
+          <t>https://s1.livelib.ru/boocover/1002688107/70/e2c6/Federiko_Aksat__Poslednij_shans.jpg</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
         <is>
-          <t>Сверхъестественное. Книга монстров, призраков, демонов и оживших мертвецов</t>
+          <t>Wizard and Glass</t>
         </is>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>Алекс Ирвин</t>
+          <t>Stephen King</t>
         </is>
       </c>
       <c r="C211" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D211" t="inlineStr"/>
       <c r="E211" t="inlineStr"/>
       <c r="F211" t="inlineStr">
         <is>
-          <t>2020 сентябрь</t>
+          <t>2020 октябрь</t>
         </is>
       </c>
       <c r="G211" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/author/219593</t>
+          <t>https://livelib.ru/author/48</t>
         </is>
       </c>
       <c r="H211" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/book/1004719459</t>
+          <t>https://livelib.ru/book/1001001100</t>
         </is>
       </c>
       <c r="I211" s="2" t="inlineStr"/>
       <c r="J211" t="n">
-        <v>4.21</v>
+        <v>4.47</v>
       </c>
       <c r="K211" s="2" t="inlineStr"/>
       <c r="L211" s="2" t="inlineStr">
         <is>
-          <t>https://s1.livelib.ru/boocover/1004719459/70/1b0c/Aleks_Irvin__Sverhestestvennoe._Kniga_monstrov_prizrakov_demonov_i_ozhivshih_mer.jpg</t>
+          <t>https://s1.livelib.ru/boocover/1001001100/70/dc68/Stephen_King__Wizard_and_Glass.jpg</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
         <is>
-          <t>Энглби</t>
+          <t>Сверхъестественное. Книга монстров, призраков, демонов и оживших мертвецов</t>
         </is>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>Себастьян Фолкс</t>
+          <t>Алекс Ирвин</t>
         </is>
       </c>
       <c r="C212" t="n">
-        <v>2.5</v>
+        <v>4</v>
       </c>
       <c r="D212" t="inlineStr"/>
       <c r="E212" t="inlineStr"/>
@@ -9371,38 +9371,38 @@
       </c>
       <c r="G212" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/author/227488</t>
+          <t>https://livelib.ru/author/219593</t>
         </is>
       </c>
       <c r="H212" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/book/1002729886</t>
+          <t>https://livelib.ru/book/1004719459</t>
         </is>
       </c>
       <c r="I212" s="2" t="inlineStr"/>
       <c r="J212" t="n">
-        <v>3.72</v>
+        <v>4.2</v>
       </c>
       <c r="K212" s="2" t="inlineStr"/>
       <c r="L212" s="2" t="inlineStr">
         <is>
-          <t>https://s1.livelib.ru/boocover/1002729886/70/10dd/Sebastyan_Folks__Englbi.jpg</t>
+          <t>https://s1.livelib.ru/boocover/1004719459/70/1b0c/Aleks_Irvin__Sverhestestvennoe._Kniga_monstrov_prizrakov_demonov_i_ozhivshih_mer.jpg</t>
         </is>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
         <is>
-          <t>Крик</t>
+          <t>The Waste Lands</t>
         </is>
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>Николя Бёгле</t>
+          <t>Stephen King</t>
         </is>
       </c>
       <c r="C213" t="n">
-        <v>2.5</v>
+        <v>5</v>
       </c>
       <c r="D213" t="inlineStr"/>
       <c r="E213" t="inlineStr"/>
@@ -9413,122 +9413,122 @@
       </c>
       <c r="G213" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/author/1166206</t>
+          <t>https://livelib.ru/author/48</t>
         </is>
       </c>
       <c r="H213" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/book/1002884491</t>
+          <t>https://livelib.ru/book/1001001098</t>
         </is>
       </c>
       <c r="I213" s="2" t="inlineStr"/>
       <c r="J213" t="n">
-        <v>3.85</v>
+        <v>4.45</v>
       </c>
       <c r="K213" s="2" t="inlineStr"/>
       <c r="L213" s="2" t="inlineStr">
         <is>
-          <t>https://s1.livelib.ru/boocover/1002884491/70/bc88/Nikolya_Bjogle__Krik.jpg</t>
+          <t>https://s1.livelib.ru/boocover/1001001098/70/dc68/Stephen_King__The_Waste_Lands.jpg</t>
         </is>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
         <is>
-          <t>Странное воспоминание</t>
+          <t>Энглби</t>
         </is>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Артур Дрейк</t>
+          <t>Себастьян Фолкс</t>
         </is>
       </c>
       <c r="C214" t="n">
-        <v>4</v>
+        <v>2.5</v>
       </c>
       <c r="D214" t="inlineStr"/>
       <c r="E214" t="inlineStr"/>
       <c r="F214" t="inlineStr">
         <is>
-          <t>2020 август</t>
+          <t>2020 сентябрь</t>
         </is>
       </c>
       <c r="G214" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/author/1068868</t>
+          <t>https://livelib.ru/author/227488</t>
         </is>
       </c>
       <c r="H214" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/book/1002688626</t>
+          <t>https://livelib.ru/book/1002729886</t>
         </is>
       </c>
       <c r="I214" s="2" t="inlineStr"/>
       <c r="J214" t="n">
-        <v>4.16</v>
+        <v>3.72</v>
       </c>
       <c r="K214" s="2" t="inlineStr"/>
       <c r="L214" s="2" t="inlineStr">
         <is>
-          <t>https://s1.livelib.ru/boocover/1002688626/70/f193/Artur_Drejk__Strannoe_vospominanie.jpg</t>
+          <t>https://s1.livelib.ru/boocover/1002729886/70/10dd/Sebastyan_Folks__Englbi.jpg</t>
         </is>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
         <is>
-          <t>Мертвое озеро</t>
+          <t>Крик</t>
         </is>
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Рейчел Кейн</t>
+          <t>Николя Бёгле</t>
         </is>
       </c>
       <c r="C215" t="n">
-        <v>3.5</v>
+        <v>2.5</v>
       </c>
       <c r="D215" t="inlineStr"/>
       <c r="E215" t="inlineStr"/>
       <c r="F215" t="inlineStr">
         <is>
-          <t>2020 август</t>
+          <t>2020 сентябрь</t>
         </is>
       </c>
       <c r="G215" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/author/124406</t>
+          <t>https://livelib.ru/author/1166206</t>
         </is>
       </c>
       <c r="H215" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/book/1002857254</t>
+          <t>https://livelib.ru/book/1002884491</t>
         </is>
       </c>
       <c r="I215" s="2" t="inlineStr"/>
       <c r="J215" t="n">
-        <v>4.01</v>
+        <v>3.85</v>
       </c>
       <c r="K215" s="2" t="inlineStr"/>
       <c r="L215" s="2" t="inlineStr">
         <is>
-          <t>https://s1.livelib.ru/boocover/1002857254/70/005a/Rejchel_Kejn__Mertvoe_ozero.jpg</t>
+          <t>https://s1.livelib.ru/boocover/1002884491/70/bc88/Nikolya_Bjogle__Krik.jpg</t>
         </is>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
         <is>
-          <t>Ледяная принцесса</t>
+          <t>Странное воспоминание</t>
         </is>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Камилла Лэкберг</t>
+          <t>Артур Дрейк</t>
         </is>
       </c>
       <c r="C216" t="n">
-        <v>3.5</v>
+        <v>4</v>
       </c>
       <c r="D216" t="inlineStr"/>
       <c r="E216" t="inlineStr"/>
@@ -9539,76 +9539,76 @@
       </c>
       <c r="G216" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/author/294412</t>
+          <t>https://livelib.ru/author/1068868</t>
         </is>
       </c>
       <c r="H216" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/book/1000740116</t>
+          <t>https://livelib.ru/book/1002688626</t>
         </is>
       </c>
       <c r="I216" s="2" t="inlineStr"/>
       <c r="J216" t="n">
-        <v>3.89</v>
+        <v>4.16</v>
       </c>
       <c r="K216" s="2" t="inlineStr"/>
       <c r="L216" s="2" t="inlineStr">
         <is>
-          <t>https://s1.livelib.ru/boocover/1000740116/70/9cd7/Kamilla_Lekberg__Ledyanaya_printsessa.jpg</t>
+          <t>https://s1.livelib.ru/boocover/1002688626/70/f193/Artur_Drejk__Strannoe_vospominanie.jpg</t>
         </is>
       </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
         <is>
-          <t>Клык и коготь</t>
+          <t>Мертвое озеро</t>
         </is>
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Джо Уолтон</t>
+          <t>Рейчел Кейн</t>
         </is>
       </c>
       <c r="C217" t="n">
-        <v>3</v>
+        <v>3.5</v>
       </c>
       <c r="D217" t="inlineStr"/>
       <c r="E217" t="inlineStr"/>
       <c r="F217" t="inlineStr">
         <is>
-          <t>2020 июль</t>
+          <t>2020 август</t>
         </is>
       </c>
       <c r="G217" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/author/342293</t>
+          <t>https://livelib.ru/author/124406</t>
         </is>
       </c>
       <c r="H217" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/book/1003637674</t>
+          <t>https://livelib.ru/book/1002857254</t>
         </is>
       </c>
       <c r="I217" s="2" t="inlineStr"/>
       <c r="J217" t="n">
-        <v>3.94</v>
+        <v>4.01</v>
       </c>
       <c r="K217" s="2" t="inlineStr"/>
       <c r="L217" s="2" t="inlineStr">
         <is>
-          <t>https://s1.livelib.ru/boocover/1003637674/70/0d35/Dzho_Uolton__Klyk_i_kogot.jpg</t>
+          <t>https://s1.livelib.ru/boocover/1002857254/70/005a/Rejchel_Kejn__Mertvoe_ozero.jpg</t>
         </is>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
         <is>
-          <t>Теллурия</t>
+          <t>Ледяная принцесса</t>
         </is>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>Владимир Сорокин</t>
+          <t>Камилла Лэкберг</t>
         </is>
       </c>
       <c r="C218" t="n">
@@ -9618,49 +9618,49 @@
       <c r="E218" t="inlineStr"/>
       <c r="F218" t="inlineStr">
         <is>
-          <t>2020 июль</t>
+          <t>2020 август</t>
         </is>
       </c>
       <c r="G218" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/author/231693</t>
+          <t>https://livelib.ru/author/294412</t>
         </is>
       </c>
       <c r="H218" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/book/1002253497</t>
+          <t>https://livelib.ru/book/1000740116</t>
         </is>
       </c>
       <c r="I218" s="2" t="inlineStr"/>
       <c r="J218" t="n">
-        <v>3.88</v>
+        <v>3.89</v>
       </c>
       <c r="K218" s="2" t="inlineStr"/>
       <c r="L218" s="2" t="inlineStr">
         <is>
-          <t>https://s1.livelib.ru/boocover/1002253497/70/e58c/Vladimir_Sorokin__Telluriya.jpg</t>
+          <t>https://s1.livelib.ru/boocover/1000740116/70/9cd7/Kamilla_Lekberg__Ledyanaya_printsessa.jpg</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
         <is>
-          <t>Бессонница</t>
+          <t>The Drawing of the Three</t>
         </is>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Стивен Кинг</t>
+          <t>Stephen King</t>
         </is>
       </c>
       <c r="C219" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="D219" t="inlineStr"/>
       <c r="E219" t="inlineStr"/>
       <c r="F219" t="inlineStr">
         <is>
-          <t>2020 октябрь</t>
+          <t>2020 август</t>
         </is>
       </c>
       <c r="G219" s="2" t="inlineStr">
@@ -9670,24 +9670,24 @@
       </c>
       <c r="H219" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/book/1000465112</t>
+          <t>https://livelib.ru/book/1001001096</t>
         </is>
       </c>
       <c r="I219" s="2" t="inlineStr"/>
       <c r="J219" t="n">
-        <v>3.97</v>
+        <v>4.47</v>
       </c>
       <c r="K219" s="2" t="inlineStr"/>
       <c r="L219" s="2" t="inlineStr">
         <is>
-          <t>https://s1.livelib.ru/boocover/1000465112/70/5b0b/Stiven_King__Bessonnitsa.jpg</t>
+          <t>https://s1.livelib.ru/boocover/1001001096/70/dc68/Stephen_King__The_Drawing_of_the_Three.jpg</t>
         </is>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
         <is>
-          <t>The Waste Lands</t>
+          <t>The Dark Tower: Gunslinger</t>
         </is>
       </c>
       <c r="B220" t="inlineStr">
@@ -9702,7 +9702,7 @@
       <c r="E220" t="inlineStr"/>
       <c r="F220" t="inlineStr">
         <is>
-          <t>2020 сентябрь</t>
+          <t>2020 июль</t>
         </is>
       </c>
       <c r="G220" s="2" t="inlineStr">
@@ -9712,75 +9712,75 @@
       </c>
       <c r="H220" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/book/1001001098</t>
+          <t>https://livelib.ru/book/1000570845</t>
         </is>
       </c>
       <c r="I220" s="2" t="inlineStr"/>
       <c r="J220" t="n">
-        <v>4.45</v>
+        <v>4.06</v>
       </c>
       <c r="K220" s="2" t="inlineStr"/>
       <c r="L220" s="2" t="inlineStr">
         <is>
-          <t>https://s1.livelib.ru/boocover/1001001098/70/dc68/Stephen_King__The_Waste_Lands.jpg</t>
+          <t>https://s1.livelib.ru/boocover/1000570845/70/903f/Stephen_King__The_Dark_Tower_Gunslinger.jpg</t>
         </is>
       </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
         <is>
-          <t>The Drawing of the Three</t>
+          <t>Клык и коготь</t>
         </is>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Stephen King</t>
+          <t>Джо Уолтон</t>
         </is>
       </c>
       <c r="C221" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D221" t="inlineStr"/>
       <c r="E221" t="inlineStr"/>
       <c r="F221" t="inlineStr">
         <is>
-          <t>2020 август</t>
+          <t>2020 июль</t>
         </is>
       </c>
       <c r="G221" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/author/48</t>
+          <t>https://livelib.ru/author/342293</t>
         </is>
       </c>
       <c r="H221" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/book/1001001096</t>
+          <t>https://livelib.ru/book/1003637674</t>
         </is>
       </c>
       <c r="I221" s="2" t="inlineStr"/>
       <c r="J221" t="n">
-        <v>4.47</v>
+        <v>3.94</v>
       </c>
       <c r="K221" s="2" t="inlineStr"/>
       <c r="L221" s="2" t="inlineStr">
         <is>
-          <t>https://s1.livelib.ru/boocover/1001001096/70/dc68/Stephen_King__The_Drawing_of_the_Three.jpg</t>
+          <t>https://s1.livelib.ru/boocover/1003637674/70/0d35/Dzho_Uolton__Klyk_i_kogot.jpg</t>
         </is>
       </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
         <is>
-          <t>The Dark Tower: Gunslinger</t>
+          <t>Теллурия</t>
         </is>
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Stephen King</t>
+          <t>Владимир Сорокин</t>
         </is>
       </c>
       <c r="C222" t="n">
-        <v>5</v>
+        <v>3.5</v>
       </c>
       <c r="D222" t="inlineStr"/>
       <c r="E222" t="inlineStr"/>
@@ -9791,22 +9791,22 @@
       </c>
       <c r="G222" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/author/48</t>
+          <t>https://livelib.ru/author/231693</t>
         </is>
       </c>
       <c r="H222" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/book/1000570845</t>
+          <t>https://livelib.ru/book/1002253497</t>
         </is>
       </c>
       <c r="I222" s="2" t="inlineStr"/>
       <c r="J222" t="n">
-        <v>4.06</v>
+        <v>3.88</v>
       </c>
       <c r="K222" s="2" t="inlineStr"/>
       <c r="L222" s="2" t="inlineStr">
         <is>
-          <t>https://s1.livelib.ru/boocover/1000570845/70/903f/Stephen_King__The_Dark_Tower_Gunslinger.jpg</t>
+          <t>https://s1.livelib.ru/boocover/1002253497/70/e58c/Vladimir_Sorokin__Telluriya.jpg</t>
         </is>
       </c>
     </row>
@@ -9847,7 +9847,7 @@
       </c>
       <c r="I223" s="2" t="inlineStr"/>
       <c r="J223" t="n">
-        <v>4</v>
+        <v>4.01</v>
       </c>
       <c r="K223" s="2" t="inlineStr"/>
       <c r="L223" s="2" t="inlineStr">
@@ -9889,7 +9889,7 @@
       </c>
       <c r="I224" s="2" t="inlineStr"/>
       <c r="J224" t="n">
-        <v>3.91</v>
+        <v>3.9</v>
       </c>
       <c r="K224" s="2" t="inlineStr"/>
       <c r="L224" s="2" t="inlineStr">
@@ -10061,7 +10061,7 @@
       </c>
       <c r="I228" s="2" t="inlineStr"/>
       <c r="J228" t="n">
-        <v>3.72</v>
+        <v>3.71</v>
       </c>
       <c r="K228" s="2" t="inlineStr"/>
       <c r="L228" s="2" t="inlineStr">
@@ -10103,7 +10103,7 @@
       </c>
       <c r="I229" s="2" t="inlineStr"/>
       <c r="J229" t="n">
-        <v>3.86</v>
+        <v>3.87</v>
       </c>
       <c r="K229" s="2" t="inlineStr"/>
       <c r="L229" s="2" t="inlineStr">
@@ -10115,100 +10115,100 @@
     <row r="230">
       <c r="A230" t="inlineStr">
         <is>
-          <t>Нью-Йоркский обход</t>
+          <t>Мизери</t>
         </is>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>Александр Стесин</t>
+          <t>Стивен Кинг</t>
         </is>
       </c>
       <c r="C230" t="n">
-        <v>2.5</v>
+        <v>4.5</v>
       </c>
       <c r="D230" t="inlineStr"/>
       <c r="E230" t="inlineStr"/>
       <c r="F230" t="inlineStr">
         <is>
-          <t>2020 май</t>
+          <t>2020 июнь</t>
         </is>
       </c>
       <c r="G230" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/author/367743</t>
+          <t>https://livelib.ru/author/48</t>
         </is>
       </c>
       <c r="H230" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/book/1003032423</t>
+          <t>https://livelib.ru/book/1000911006</t>
         </is>
       </c>
       <c r="I230" s="2" t="inlineStr"/>
       <c r="J230" t="n">
-        <v>3.76</v>
+        <v>4.47</v>
       </c>
       <c r="K230" s="2" t="inlineStr"/>
       <c r="L230" s="2" t="inlineStr">
         <is>
-          <t>https://s1.livelib.ru/boocover/1003032423/70/7a69/Aleksandr_Stesin__NyuJorkskij_obhod.jpg</t>
+          <t>https://s1.livelib.ru/boocover/1000911006/70/6b72/Stiven_King__Mizeri.jpg</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
         <is>
-          <t>Лучше, чем секс</t>
+          <t>Нью-Йоркский обход</t>
         </is>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Хантер С. Томпсон</t>
+          <t>Александр Стесин</t>
         </is>
       </c>
       <c r="C231" t="n">
-        <v>1</v>
+        <v>2.5</v>
       </c>
       <c r="D231" t="inlineStr"/>
       <c r="E231" t="inlineStr"/>
       <c r="F231" t="inlineStr">
         <is>
-          <t>2020 апрель</t>
+          <t>2020 май</t>
         </is>
       </c>
       <c r="G231" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/author/106580</t>
+          <t>https://livelib.ru/author/367743</t>
         </is>
       </c>
       <c r="H231" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/book/1000323170</t>
+          <t>https://livelib.ru/book/1003032423</t>
         </is>
       </c>
       <c r="I231" s="2" t="inlineStr"/>
       <c r="J231" t="n">
-        <v>3.62</v>
+        <v>3.77</v>
       </c>
       <c r="K231" s="2" t="inlineStr"/>
       <c r="L231" s="2" t="inlineStr">
         <is>
-          <t>https://s1.livelib.ru/boocover/1000323170/70/79b0/Hanter_S._Tompson__Luchshe_chem_seks.jpg</t>
+          <t>https://s1.livelib.ru/boocover/1003032423/70/7a69/Aleksandr_Stesin__NyuJorkskij_obhod.jpg</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
         <is>
-          <t>Белый отель</t>
+          <t>Лучше, чем секс</t>
         </is>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Дональд Майкл Томас</t>
+          <t>Хантер С. Томпсон</t>
         </is>
       </c>
       <c r="C232" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D232" t="inlineStr"/>
       <c r="E232" t="inlineStr"/>
@@ -10219,38 +10219,38 @@
       </c>
       <c r="G232" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/author/28559</t>
+          <t>https://livelib.ru/author/106580</t>
         </is>
       </c>
       <c r="H232" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/book/1000772831</t>
+          <t>https://livelib.ru/book/1000323170</t>
         </is>
       </c>
       <c r="I232" s="2" t="inlineStr"/>
       <c r="J232" t="n">
-        <v>3.79</v>
+        <v>3.62</v>
       </c>
       <c r="K232" s="2" t="inlineStr"/>
       <c r="L232" s="2" t="inlineStr">
         <is>
-          <t>https://s1.livelib.ru/boocover/1000772831/70/e48d/Donald_Majkl_Tomas__Belyj_otel.jpg</t>
+          <t>https://s1.livelib.ru/boocover/1000323170/70/79b0/Hanter_S._Tompson__Luchshe_chem_seks.jpg</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
         <is>
-          <t>Там...</t>
+          <t>Белый отель</t>
         </is>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Борис Акунин</t>
+          <t>Дональд Майкл Томас</t>
         </is>
       </c>
       <c r="C233" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D233" t="inlineStr"/>
       <c r="E233" t="inlineStr"/>
@@ -10261,38 +10261,38 @@
       </c>
       <c r="G233" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/author/173873</t>
+          <t>https://livelib.ru/author/28559</t>
         </is>
       </c>
       <c r="H233" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/book/1000393484</t>
+          <t>https://livelib.ru/book/1000772831</t>
         </is>
       </c>
       <c r="I233" s="2" t="inlineStr"/>
       <c r="J233" t="n">
-        <v>3.72</v>
+        <v>3.79</v>
       </c>
       <c r="K233" s="2" t="inlineStr"/>
       <c r="L233" s="2" t="inlineStr">
         <is>
-          <t>https://s1.livelib.ru/boocover/1000393484/70/fae2/__Tam....jpg</t>
+          <t>https://s1.livelib.ru/boocover/1000772831/70/e48d/Donald_Majkl_Tomas__Belyj_otel.jpg</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
         <is>
-          <t>Шкура</t>
+          <t>Там...</t>
         </is>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Юлия Волкодав</t>
+          <t>Борис Акунин</t>
         </is>
       </c>
       <c r="C234" t="n">
-        <v>3.5</v>
+        <v>3</v>
       </c>
       <c r="D234" t="inlineStr"/>
       <c r="E234" t="inlineStr"/>
@@ -10303,80 +10303,80 @@
       </c>
       <c r="G234" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/author/838773</t>
+          <t>https://livelib.ru/author/173873</t>
         </is>
       </c>
       <c r="H234" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/book/1002707902</t>
+          <t>https://livelib.ru/book/1000393484</t>
         </is>
       </c>
       <c r="I234" s="2" t="inlineStr"/>
       <c r="J234" t="n">
-        <v>4.19</v>
+        <v>3.72</v>
       </c>
       <c r="K234" s="2" t="inlineStr"/>
       <c r="L234" s="2" t="inlineStr">
         <is>
-          <t>https://s1.livelib.ru/boocover/1002707902/70/e84f/Yuliya_Volkodav__Shkura.jpg</t>
+          <t>https://s1.livelib.ru/boocover/1000393484/70/fae2/__Tam....jpg</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
         <is>
-          <t>Тринадцатая сказка</t>
+          <t>Шкура</t>
         </is>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Диана Сеттерфилд</t>
+          <t>Юлия Волкодав</t>
         </is>
       </c>
       <c r="C235" t="n">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="D235" t="inlineStr"/>
       <c r="E235" t="inlineStr"/>
       <c r="F235" t="inlineStr">
         <is>
-          <t>2020 март</t>
+          <t>2020 апрель</t>
         </is>
       </c>
       <c r="G235" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/author/198413</t>
+          <t>https://livelib.ru/author/838773</t>
         </is>
       </c>
       <c r="H235" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/book/1000691691</t>
+          <t>https://livelib.ru/book/1002707902</t>
         </is>
       </c>
       <c r="I235" s="2" t="inlineStr"/>
       <c r="J235" t="n">
-        <v>4.31</v>
+        <v>4.18</v>
       </c>
       <c r="K235" s="2" t="inlineStr"/>
       <c r="L235" s="2" t="inlineStr">
         <is>
-          <t>https://s1.livelib.ru/boocover/1000691691/70/2e61/Diana_Setterfild__Trinadtsataya_skazka.jpg</t>
+          <t>https://s1.livelib.ru/boocover/1002707902/70/e84f/Yuliya_Volkodav__Shkura.jpg</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
         <is>
-          <t>Дверь</t>
+          <t>Тринадцатая сказка</t>
         </is>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Магда Сабо</t>
+          <t>Диана Сеттерфилд</t>
         </is>
       </c>
       <c r="C236" t="n">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="D236" t="inlineStr"/>
       <c r="E236" t="inlineStr"/>
@@ -10387,38 +10387,38 @@
       </c>
       <c r="G236" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/author/303379</t>
+          <t>https://livelib.ru/author/198413</t>
         </is>
       </c>
       <c r="H236" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/book/1002976462</t>
+          <t>https://livelib.ru/book/1000691691</t>
         </is>
       </c>
       <c r="I236" s="2" t="inlineStr"/>
       <c r="J236" t="n">
-        <v>4.05</v>
+        <v>4.31</v>
       </c>
       <c r="K236" s="2" t="inlineStr"/>
       <c r="L236" s="2" t="inlineStr">
         <is>
-          <t>https://s1.livelib.ru/boocover/1002976462/70/bb30/Magda_Sabo__Dver.jpg</t>
+          <t>https://s1.livelib.ru/boocover/1000691691/70/2e61/Diana_Setterfild__Trinadtsataya_skazka.jpg</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
         <is>
-          <t>Порою блажь великая</t>
+          <t>Дверь</t>
         </is>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Кен Кизи</t>
+          <t>Магда Сабо</t>
         </is>
       </c>
       <c r="C237" t="n">
-        <v>4</v>
+        <v>4.5</v>
       </c>
       <c r="D237" t="inlineStr"/>
       <c r="E237" t="inlineStr"/>
@@ -10429,38 +10429,38 @@
       </c>
       <c r="G237" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/author/182918</t>
+          <t>https://livelib.ru/author/303379</t>
         </is>
       </c>
       <c r="H237" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/book/1002753975</t>
+          <t>https://livelib.ru/book/1002976462</t>
         </is>
       </c>
       <c r="I237" s="2" t="inlineStr"/>
       <c r="J237" t="n">
-        <v>4.35</v>
+        <v>4.05</v>
       </c>
       <c r="K237" s="2" t="inlineStr"/>
       <c r="L237" s="2" t="inlineStr">
         <is>
-          <t>https://s1.livelib.ru/boocover/1002753975/70/144b/Ken_Kizi__Poroyu_blazh_velikaya.jpg</t>
+          <t>https://s1.livelib.ru/boocover/1002976462/70/bb30/Magda_Sabo__Dver.jpg</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
         <is>
-          <t>Зелёная миля</t>
+          <t>Порою блажь великая</t>
         </is>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Стивен Кинг</t>
+          <t>Кен Кизи</t>
         </is>
       </c>
       <c r="C238" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D238" t="inlineStr"/>
       <c r="E238" t="inlineStr"/>
@@ -10471,38 +10471,38 @@
       </c>
       <c r="G238" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/author/48</t>
+          <t>https://livelib.ru/author/182918</t>
         </is>
       </c>
       <c r="H238" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/book/1000966838</t>
+          <t>https://livelib.ru/book/1002753975</t>
         </is>
       </c>
       <c r="I238" s="2" t="inlineStr"/>
       <c r="J238" t="n">
-        <v>4.72</v>
+        <v>4.35</v>
       </c>
       <c r="K238" s="2" t="inlineStr"/>
       <c r="L238" s="2" t="inlineStr">
         <is>
-          <t>https://s1.livelib.ru/boocover/1000966838/70/7df1/Stiven_King__Zeljonaya_milya.jpg</t>
+          <t>https://s1.livelib.ru/boocover/1002753975/70/144b/Ken_Kizi__Poroyu_blazh_velikaya.jpg</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
         <is>
-          <t>Дитя подвала</t>
+          <t>Зелёная миля</t>
         </is>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>Александр Варго</t>
+          <t>Стивен Кинг</t>
         </is>
       </c>
       <c r="C239" t="n">
-        <v>3.5</v>
+        <v>5</v>
       </c>
       <c r="D239" t="inlineStr"/>
       <c r="E239" t="inlineStr"/>
@@ -10513,34 +10513,34 @@
       </c>
       <c r="G239" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/author/227311</t>
+          <t>https://livelib.ru/author/48</t>
         </is>
       </c>
       <c r="H239" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/book/1002954049</t>
+          <t>https://livelib.ru/book/1000966838</t>
         </is>
       </c>
       <c r="I239" s="2" t="inlineStr"/>
       <c r="J239" t="n">
-        <v>3.42</v>
+        <v>4.71</v>
       </c>
       <c r="K239" s="2" t="inlineStr"/>
       <c r="L239" s="2" t="inlineStr">
         <is>
-          <t>https://s1.livelib.ru/boocover/1002954049/70/d139/Aleksandr_Vargo__Ditya_podvala.jpg</t>
+          <t>https://s1.livelib.ru/boocover/1000966838/70/7df1/Stiven_King__Zeljonaya_milya.jpg</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
         <is>
-          <t>Врата Анубиса</t>
+          <t>Дитя подвала</t>
         </is>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Тим Пауэрс</t>
+          <t>Александр Варго</t>
         </is>
       </c>
       <c r="C240" t="n">
@@ -10555,38 +10555,38 @@
       </c>
       <c r="G240" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/author/101499</t>
+          <t>https://livelib.ru/author/227311</t>
         </is>
       </c>
       <c r="H240" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/book/1000086632</t>
+          <t>https://livelib.ru/book/1002954049</t>
         </is>
       </c>
       <c r="I240" s="2" t="inlineStr"/>
       <c r="J240" t="n">
-        <v>3.82</v>
+        <v>3.42</v>
       </c>
       <c r="K240" s="2" t="inlineStr"/>
       <c r="L240" s="2" t="inlineStr">
         <is>
-          <t>https://s1.livelib.ru/boocover/1000086632/70/5066/Tim_Pauers__Vrata_Anubisa.jpg</t>
+          <t>https://s1.livelib.ru/boocover/1002954049/70/d139/Aleksandr_Vargo__Ditya_podvala.jpg</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
         <is>
-          <t>Когда дым застилает глаза. Провокационные истории о своей любимой работе от сотрудника крематория</t>
+          <t>Врата Анубиса</t>
         </is>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Кейтлин Даути</t>
+          <t>Тим Пауэрс</t>
         </is>
       </c>
       <c r="C241" t="n">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="D241" t="inlineStr"/>
       <c r="E241" t="inlineStr"/>
@@ -10597,64 +10597,64 @@
       </c>
       <c r="G241" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/author/1085673</t>
+          <t>https://livelib.ru/author/101499</t>
         </is>
       </c>
       <c r="H241" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/book/1002746376</t>
+          <t>https://livelib.ru/book/1000086632</t>
         </is>
       </c>
       <c r="I241" s="2" t="inlineStr"/>
       <c r="J241" t="n">
-        <v>4.06</v>
+        <v>3.82</v>
       </c>
       <c r="K241" s="2" t="inlineStr"/>
       <c r="L241" s="2" t="inlineStr">
         <is>
-          <t>https://s1.livelib.ru/boocover/1002746376/70/bee8/Kejtlin_Dauti__Kogda_dym_zastilaet_glaza._Provokatsionnye_istorii_o_svoej_lyubim.jpg</t>
+          <t>https://s1.livelib.ru/boocover/1000086632/70/5066/Tim_Pauers__Vrata_Anubisa.jpg</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
         <is>
-          <t>Мизери</t>
+          <t>Когда дым застилает глаза. Провокационные истории о своей любимой работе от сотрудника крематория</t>
         </is>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Стивен Кинг</t>
+          <t>Кейтлин Даути</t>
         </is>
       </c>
       <c r="C242" t="n">
-        <v>4.5</v>
+        <v>4</v>
       </c>
       <c r="D242" t="inlineStr"/>
       <c r="E242" t="inlineStr"/>
       <c r="F242" t="inlineStr">
         <is>
-          <t>2020 июнь</t>
+          <t>2020 март</t>
         </is>
       </c>
       <c r="G242" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/author/48</t>
+          <t>https://livelib.ru/author/1085673</t>
         </is>
       </c>
       <c r="H242" s="2" t="inlineStr">
         <is>
-          <t>https://livelib.ru/book/1000911006</t>
+          <t>https://livelib.ru/book/1002746376</t>
         </is>
       </c>
       <c r="I242" s="2" t="inlineStr"/>
       <c r="J242" t="n">
-        <v>4.47</v>
+        <v>4.06</v>
       </c>
       <c r="K242" s="2" t="inlineStr"/>
       <c r="L242" s="2" t="inlineStr">
         <is>
-          <t>https://s1.livelib.ru/boocover/1000911006/70/6b72/Stiven_King__Mizeri.jpg</t>
+          <t>https://s1.livelib.ru/boocover/1002746376/70/bee8/Kejtlin_Dauti__Kogda_dym_zastilaet_glaza._Provokatsionnye_istorii_o_svoej_lyubim.jpg</t>
         </is>
       </c>
     </row>
@@ -11061,7 +11061,7 @@
       </c>
       <c r="I252" s="2" t="inlineStr"/>
       <c r="J252" t="n">
-        <v>3.87</v>
+        <v>3.88</v>
       </c>
       <c r="K252" s="2" t="inlineStr"/>
       <c r="L252" s="2" t="inlineStr">
@@ -11229,7 +11229,7 @@
       </c>
       <c r="I256" s="2" t="inlineStr"/>
       <c r="J256" t="n">
-        <v>4.14</v>
+        <v>4.13</v>
       </c>
       <c r="K256" s="2" t="inlineStr"/>
       <c r="L256" s="2" t="inlineStr">
@@ -11313,7 +11313,7 @@
       </c>
       <c r="I258" s="2" t="inlineStr"/>
       <c r="J258" t="n">
-        <v>3.55</v>
+        <v>3.56</v>
       </c>
       <c r="K258" s="2" t="inlineStr"/>
       <c r="L258" s="2" t="inlineStr">
@@ -11355,7 +11355,7 @@
       </c>
       <c r="I259" s="2" t="inlineStr"/>
       <c r="J259" t="n">
-        <v>4.33</v>
+        <v>4.32</v>
       </c>
       <c r="K259" s="2" t="inlineStr"/>
       <c r="L259" s="2" t="inlineStr">
@@ -11397,7 +11397,7 @@
       </c>
       <c r="I260" s="2" t="inlineStr"/>
       <c r="J260" t="n">
-        <v>4.57</v>
+        <v>4.58</v>
       </c>
       <c r="K260" s="2" t="inlineStr"/>
       <c r="L260" s="2" t="inlineStr">
@@ -11607,7 +11607,7 @@
       </c>
       <c r="I265" s="2" t="inlineStr"/>
       <c r="J265" t="n">
-        <v>3.63</v>
+        <v>3.64</v>
       </c>
       <c r="K265" s="2" t="inlineStr"/>
       <c r="L265" s="2" t="inlineStr">
@@ -11779,7 +11779,7 @@
       </c>
       <c r="I269" s="2" t="inlineStr"/>
       <c r="J269" t="n">
-        <v>3.81</v>
+        <v>3.79</v>
       </c>
       <c r="K269" s="2" t="inlineStr"/>
       <c r="L269" s="2" t="inlineStr">
@@ -12920,7 +12920,7 @@
       </c>
       <c r="I296" s="2" t="inlineStr"/>
       <c r="J296" t="n">
-        <v>3.34</v>
+        <v>3.33</v>
       </c>
       <c r="K296" s="2" t="inlineStr"/>
       <c r="L296" s="2" t="inlineStr">
@@ -13088,7 +13088,7 @@
       </c>
       <c r="I300" s="2" t="inlineStr"/>
       <c r="J300" t="n">
-        <v>3.89</v>
+        <v>3.88</v>
       </c>
       <c r="K300" s="2" t="inlineStr"/>
       <c r="L300" s="2" t="inlineStr">
@@ -13210,7 +13210,7 @@
       </c>
       <c r="I303" s="2" t="inlineStr"/>
       <c r="J303" t="n">
-        <v>3.58</v>
+        <v>3.56</v>
       </c>
       <c r="K303" s="2" t="inlineStr"/>
       <c r="L303" s="2" t="inlineStr">
@@ -13336,7 +13336,7 @@
       </c>
       <c r="I306" s="2" t="inlineStr"/>
       <c r="J306" t="n">
-        <v>3.61</v>
+        <v>3.63</v>
       </c>
       <c r="K306" s="2" t="inlineStr"/>
       <c r="L306" s="2" t="inlineStr">
@@ -13630,7 +13630,7 @@
       </c>
       <c r="I313" s="2" t="inlineStr"/>
       <c r="J313" t="n">
-        <v>3.69</v>
+        <v>3.68</v>
       </c>
       <c r="K313" s="2" t="inlineStr"/>
       <c r="L313" s="2" t="inlineStr">
@@ -13672,7 +13672,7 @@
       </c>
       <c r="I314" s="2" t="inlineStr"/>
       <c r="J314" t="n">
-        <v>4.05</v>
+        <v>4.04</v>
       </c>
       <c r="K314" s="2" t="inlineStr"/>
       <c r="L314" s="2" t="inlineStr">
@@ -13832,7 +13832,7 @@
       </c>
       <c r="I318" s="2" t="inlineStr"/>
       <c r="J318" t="n">
-        <v>3.39</v>
+        <v>3.38</v>
       </c>
       <c r="K318" s="2" t="inlineStr"/>
       <c r="L318" s="2" t="inlineStr">
@@ -14219,7 +14219,7 @@
       </c>
       <c r="I327" s="2" t="inlineStr"/>
       <c r="J327" t="n">
-        <v>4.3</v>
+        <v>4.29</v>
       </c>
       <c r="K327" s="2" t="inlineStr"/>
       <c r="L327" s="2" t="inlineStr">
@@ -14334,12 +14334,7 @@
 Кирилл спешит на свидание к своей девушке Алисе, которая готовит ему сюрприз в лесопарке. Внезапно она ему звонит и говорит, что видит незнакомого мужчину. Кирилл не особо в это верит и считает, что это прелюдия к хорошему вечеру. А затем происходят вещи, про которые нужно читать.
 Сюжет прост, но то, как автор расписывает уходящие секунды до встречи, нервное напряжение Кирилла, ожидание и надежду Алисы.. всё это поражает достоверностью происходящего. Хочешь не хочешь, а задумаешься о быстротечности времени и о том, что пару мгновений могут изменить всё. И еще, я до ужаса боюсь вещей, которые происходят в городских реалиях. Моя мнительность зашкаливает. Плюс автору.10/10.
 ПОЩЕЧИНА. АНДРЕЙ ФРОЛОВ. Этот автор мне знаком своими рассказами "Пунктирный" и "Шлепушка". Я от них в восторге, эта история меня также не разочаровала.
-Перспективный актер начинает работу в другом театре. Там его ждёт новый коллектив с устоявшимися привычками и приобретенными суевериями, а наш главный герой решает "войти в чужой монастырь со своим уставом". Ничего хорошего из этого не выходит.
-Крови немного, мистика в пределах разумного, погружение стопроцентное, такое ощущение, что вместе с героем стоишь на театральных подмостках и играешь роль. 9/10.
-ДВА ХИЩНЫХ ВЗГЛЯДА. АНДРЕЙ ФРОЛОВ. Популярный блогер Ирэн решила в срочном порядке снять деньги из банкомата. Стремглав помчавшись на поиски оного она находит нечто. А в довесок к странному нечто добавляются два одетых в спортивки молодых человека.
-Крови чуть больше, напряжение к финалу нарастает, невероятность событий зашкаливает. 9/10.
-Эти рассказы Фролова немного напоминают раннего Стивена Кинга, который любил наделять неодушевленные предметы демонической душой. Это не раздражает, так как Фролов мастерски использует данный прием, примеряя его на нашу повседневность. Молодец.
-В целом, я сборником довольна, неудачная повесть не испортила впечатление. Если будете читать можете ее смело пропустить и приступить сразу к рассказам. Большого количества кровищи в них вы не найдете, а вот читая повесть нужно будет примерить "Красные перчатки", привет Ллойду.</t>
+Перспективный актер начинает работу в другом театре. Там его ждёт новый коллектив с устоявшимися прив</t>
         </is>
       </c>
       <c r="E330" s="3" t="inlineStr"/>
@@ -14448,7 +14443,7 @@
       </c>
       <c r="I332" s="2" t="inlineStr"/>
       <c r="J332" t="n">
-        <v>4.11</v>
+        <v>4.1</v>
       </c>
       <c r="K332" s="2" t="inlineStr"/>
       <c r="L332" s="2" t="inlineStr">
@@ -14873,7 +14868,7 @@
       </c>
       <c r="I342" s="2" t="inlineStr"/>
       <c r="J342" t="n">
-        <v>4.07</v>
+        <v>4.05</v>
       </c>
       <c r="K342" s="2" t="inlineStr"/>
       <c r="L342" s="2" t="inlineStr">
@@ -15375,7 +15370,7 @@
       </c>
       <c r="I353" s="2" t="inlineStr"/>
       <c r="J353" t="n">
-        <v>3.51</v>
+        <v>3.5</v>
       </c>
       <c r="K353" s="2" t="inlineStr"/>
       <c r="L353" s="2" t="inlineStr">
@@ -15426,7 +15421,7 @@
       </c>
       <c r="I354" s="5" t="inlineStr"/>
       <c r="J354" s="3" t="n">
-        <v>3.44</v>
+        <v>3.43</v>
       </c>
       <c r="K354" s="5" t="inlineStr">
         <is>
@@ -15942,7 +15937,7 @@
       </c>
       <c r="I365" s="2" t="inlineStr"/>
       <c r="J365" t="n">
-        <v>3.21</v>
+        <v>3.2</v>
       </c>
       <c r="K365" s="2" t="inlineStr"/>
       <c r="L365" s="2" t="inlineStr">
@@ -15984,7 +15979,7 @@
       </c>
       <c r="I366" s="2" t="inlineStr"/>
       <c r="J366" t="n">
-        <v>3.96</v>
+        <v>3.97</v>
       </c>
       <c r="K366" s="2" t="inlineStr"/>
       <c r="L366" s="2" t="inlineStr">
@@ -16457,9 +16452,7 @@
 1. Неадекват. Написал пресловутый Сергей Демин, автор книг "Кристмас", "Льдинка", "Дикий пляж", "Дом в овраге" и т.д. Рассказ об уголовнике, который ищет проститутку, чтобы ей отомстить. Полный трэш. В духе Демина, но мне не понравилось, так как это смахивает на мало бюджетный фильм с кучей дешевых штампов.
 2. Слухи. Написал Максим Кабир. Лучшее, что есть в этом сборнике. Три гадкие бабки сидят на лавочке перед подъездом и чешут языками. Всё, что они говорят сбывается. Хоть это и рассказ, но погружение моментальное. 10 из 10 однозначно.
 3. Яма на дне колодца. Это роман, который я приняла за рассказы. Написал Андрей Фролов. Есть некий Особняк, в котором живет обычная семья вампиров. Они не боятся солнечного цвета, отражаются в зеркалах, чеснок уплетают за обе щеки и не чураются человеческой еды. Но у каждого вампира есть свои потребности и Особняк им в этом помогает. Он "притягивает" людей. Схема такова: под видом обеспеченной семьи вампиры нанимают на работу "бедолаг" для того, чтобы они ухаживали за домом - убирали, готовили, чинили. Они хорошо платят своей "еде", вкусно ее кормят и не выпускают из Особняка. Никто, если честно, и не рвется на волю. Кроме главного героя.
-Начну с объективных плюсов: написано хорошо, сюжет продуман, подробно прописаны чувства главного героя и физиология. В книге нет хэппиэнда. Атрибуты жанра соблюдены.
-Объективных минусов я не увидела, но мне книга не понравилась. Меня не зацепили метания героя. Хотелось сказать: "Соберись, тряпка!". Раздражали фразы что-то типа: "Я пролежень на отмершей ноге старика, забытого в больничном коридоре" или "Я натянутая кожа мертвеца, задушенного рояльной струной". Меня не покидало чувство, что я уже где-то это видела. Ну да, "Бойцовский клуб". Я не читала Паланика вообще, но я смотрела фильм, и да "Я ухмыляющаяся месть Джека". Не надо так. Внезапно метания прекратились и начались упоминания про твиттер и хэштэги. Это вилы.
-В общем, сборник неплохой, последний роман может быть достойно оценён любителями Паланика, наверное. Я не знаю.</t>
+Начну с объективных плюсов: написано хорошо, сюжет продуман, подробно про</t>
         </is>
       </c>
       <c r="E377" s="3" t="inlineStr"/>
@@ -16518,7 +16511,7 @@
       </c>
       <c r="I378" s="2" t="inlineStr"/>
       <c r="J378" t="n">
-        <v>3.53</v>
+        <v>3.56</v>
       </c>
       <c r="K378" s="2" t="inlineStr"/>
       <c r="L378" s="2" t="inlineStr">
@@ -16560,7 +16553,7 @@
       </c>
       <c r="I379" s="2" t="inlineStr"/>
       <c r="J379" t="n">
-        <v>3.65</v>
+        <v>3.66</v>
       </c>
       <c r="K379" s="2" t="inlineStr"/>
       <c r="L379" s="2" t="inlineStr">
@@ -16751,7 +16744,7 @@
       </c>
       <c r="I383" s="5" t="inlineStr"/>
       <c r="J383" s="3" t="n">
-        <v>2.54</v>
+        <v>2.56</v>
       </c>
       <c r="K383" s="5" t="inlineStr">
         <is>
@@ -17007,7 +17000,7 @@
       </c>
       <c r="I389" s="2" t="inlineStr"/>
       <c r="J389" t="n">
-        <v>3.41</v>
+        <v>3.42</v>
       </c>
       <c r="K389" s="2" t="inlineStr"/>
       <c r="L389" s="2" t="inlineStr">
@@ -17434,7 +17427,7 @@
       </c>
       <c r="I399" s="5" t="inlineStr"/>
       <c r="J399" s="3" t="n">
-        <v>3.99</v>
+        <v>3.94</v>
       </c>
       <c r="K399" s="5" t="inlineStr">
         <is>
@@ -17564,7 +17557,7 @@
       </c>
       <c r="I402" s="2" t="inlineStr"/>
       <c r="J402" t="n">
-        <v>4.38</v>
+        <v>4.37</v>
       </c>
       <c r="K402" s="2" t="inlineStr"/>
       <c r="L402" s="2" t="inlineStr">
@@ -17648,7 +17641,7 @@
       </c>
       <c r="I404" s="2" t="inlineStr"/>
       <c r="J404" t="n">
-        <v>3.56</v>
+        <v>3.57</v>
       </c>
       <c r="K404" s="2" t="inlineStr"/>
       <c r="L404" s="2" t="inlineStr">
@@ -18365,7 +18358,7 @@
       </c>
       <c r="I420" s="2" t="inlineStr"/>
       <c r="J420" t="n">
-        <v>3.74</v>
+        <v>3.73</v>
       </c>
       <c r="K420" s="2" t="inlineStr"/>
       <c r="L420" s="2" t="inlineStr">
@@ -19396,7 +19389,7 @@
       </c>
       <c r="I444" s="2" t="inlineStr"/>
       <c r="J444" t="n">
-        <v>3.58</v>
+        <v>3.59</v>
       </c>
       <c r="K444" s="2" t="inlineStr"/>
       <c r="L444" s="2" t="inlineStr">
@@ -19550,8 +19543,7 @@
           <t>Это был обычный пикник возле обычного дома в пригороде Мельбурна, на котором собрались совсем обычные люди. И ничто не предвещало того, что совсем скоро случится то, что случилось. Один из гостей, взбешенный поведением чужого трехлетнего ребенка, отвешивает ему полновесную пощечину. И тут понеслась...
 Помимо того, что эту книгу признали лучшей в Австралии, долгое время она числилась в списке национальных бестселлеров, так она еще и прославила автора. Прочитав её я понимаю почему. Здесь есть всё: наркотики, откровенные постельные сцены, измены, интрижки, геи, долбанутый на всю голову персонаж, остросоциальные темы, и конечно же, постоянный вопрос от автора: на чьей ты стороне? Лично я не выбираю ни одну из сторон, я просто не осуждаю мужика за то, что он сделал. Да, он ударил ребенка, но у него была на это веская причина. Да, он должен был тысячу раз подумать прежде чем решиться и ударить избалованного ребенка, но у него на это была веская причина, и если родители этого ребенка просто предпочли закрыть глаза на его (ребенка) поведение, то мужик не закрыл, потому что у него на это была веская причина.
 Как же меня бомбило от осознания того, что есть такие яжматери и в настоящей жизни. Как же они своим наседством раздражают. Уймитесь, дамочки,  вред собственному ребенку причиняете только вы своей гиперопекой, неспособностью объяснить ребенку, что такое хорошо, а что такое плохо. Вы своими куриными мозгами не понимаете, что ребенок должен познавать мир сам, он должен ошибаться и учиться, радоваться и огорчаться. Сам. Ваша задача быть опорой и твёрдой, но ненавязчивой рукой, которая направит на путь истинный, если что, а не вакуумом в котором все позволено.  В общем, одна из героинь была именно такой.  И еще, добью вас. Она давала грудь своему трехлетнему сыну!!! Тупая пи**а!!! Как так-то??
-Наш менталитет от австралийского кардинально отличается. Если ты  ударил ребёнка там, то это капец какая трагедия. Если шкодит ребенок у нас, он получает по жопе и всё.
-Я бы не назвала эту книгу бестселлером года, мне казалось, что чего-то не хватает, что сюжет должен был пойти по совсем другой траектории, но с большего книга мне понравилась. Она показала, в очередной раз, что и такое может быть. За тему книги - плюс, за тупых персонажей - жирнейший минус.</t>
+Наш менталитет от австралийского кардинально отличается</t>
         </is>
       </c>
       <c r="E448" s="3" t="inlineStr"/>
@@ -19572,7 +19564,7 @@
       </c>
       <c r="I448" s="5" t="inlineStr"/>
       <c r="J448" s="3" t="n">
-        <v>3.59</v>
+        <v>3.6</v>
       </c>
       <c r="K448" s="5" t="inlineStr">
         <is>
@@ -19989,7 +19981,7 @@
 Вас ждет средневековая Россия 15 века, поэтому язык здесь не только современный, но и древнерусский. Книга написана в жанре роман-житие и  поэтому огромное количество философских разговоров, наставлений, нравоучений обязательны. На каждой странице вас ждет косвенное или прямое упоминание Бога. Он во всем: в травинке, в калаче, в реке, в тебе. Везде. Вы однозначно прочувствуете весь спектр эмоций и не останетесь равнодушными. 
 А вот теперь субъективное мнение. Чем больше времени проходит с момента прочтения последней страницы,  тем больше во мне растет неприятие этой книги. Первым толчком послужило выдергивание из атмосферы средневековья. Сейчас объясню. Я вместе с героем нахожусь в лесу, наблюдаю как зима отступает, а весна входит в свои права, просыпается жизнь, тает снег, а под ним и прошлогодние листья, и обрывки тряпок, и пластиковые бутылки. Как так-то???????? Я выпала в осадок на 15 минут!! У меня был шок, почему этот ляп пропустили в печать? Зачем автор так сделал? И первой мыслью было захлопнуть книгу и больше к ней не притрагиваться. Когда оцепенение прошло, я подумала,  что это фишка автора и нужно дочитать до конца. Что я и сделала. Но дальше меня ждал еще один сюрприз, правда не такой грандиозный как бутылки, но было немного дико. Смешение языков. В одном предложении вы встретите как церковно славянские фразы так и матерный сленг. Так вот, дочитала книгу и не обнаружила ничего.
 Любезный интернет предоставил мне полезную информацию. Сам автор дает разъяснение касательно появления этих чертовых пластиковых бутылок. Они, как бЭ, указывают на отсутствие времени. Отсюда и они, и смешение языков,  и наши современные замашки. Так что это не ляп, это ход, который показывает, что время не имеет границ. Если времени нет, тогда зачем указывать, что это 15 век? Если бы Арсений был попаданцем, то бутылки, мат были бы кстати)) и еще вопрос, почему Арсений решил,  что сможет спасти душу Устины? В чем его вина? В наше время, до его поступка никому нет дела, а вот в 15 веке - это действительно страшно. То есть еще одно указание на конкретное время. В общем, сам автор сказал, что в следующей редакции эти моменты уберут.
-В общем,  мне не понравилось. Бутылки сделали свое дело. За всем этим я не смогла по достоинству оценить ту доброту, жертвенность, мудрость, которые автор заложил в героя, не оценила победу духа над телом, не рассмотрела все те старые, но хорошо известные истины, а главное не прочувствовала всю глубину веры и духовности, которыми наполнена книга. Язык изложения отличный, а вот подача меня смутила.</t>
+В общем,  мне не понравилось. Бутылки сделали свое дело. За всем этим я не смогла по достоинству оценить ту доброту, жертвенность, мудрость, которые автор заложил в героя, не оценила победу духа над телом, не рассмотрела все те старые, но хорошо известные истины, а главное не прочувств</t>
         </is>
       </c>
       <c r="E458" s="3" t="inlineStr"/>
@@ -20560,7 +20552,7 @@
       </c>
       <c r="I471" s="2" t="inlineStr"/>
       <c r="J471" t="n">
-        <v>3.5</v>
+        <v>3.48</v>
       </c>
       <c r="K471" s="2" t="inlineStr"/>
       <c r="L471" s="2" t="inlineStr">
@@ -20770,7 +20762,7 @@
       </c>
       <c r="I476" s="2" t="inlineStr"/>
       <c r="J476" t="n">
-        <v>4.18</v>
+        <v>4.17</v>
       </c>
       <c r="K476" s="2" t="inlineStr"/>
       <c r="L476" s="2" t="inlineStr">
@@ -20812,7 +20804,7 @@
       </c>
       <c r="I477" s="2" t="inlineStr"/>
       <c r="J477" t="n">
-        <v>3.66</v>
+        <v>3.65</v>
       </c>
       <c r="K477" s="2" t="inlineStr"/>
       <c r="L477" s="2" t="inlineStr">
@@ -21148,7 +21140,7 @@
       </c>
       <c r="I485" s="2" t="inlineStr"/>
       <c r="J485" t="n">
-        <v>4.13</v>
+        <v>4.12</v>
       </c>
       <c r="K485" s="2" t="inlineStr"/>
       <c r="L485" s="2" t="inlineStr">
@@ -21568,7 +21560,7 @@
       </c>
       <c r="I495" s="2" t="inlineStr"/>
       <c r="J495" t="n">
-        <v>3.1</v>
+        <v>3.11</v>
       </c>
       <c r="K495" s="2" t="inlineStr"/>
       <c r="L495" s="2" t="inlineStr">
@@ -21854,7 +21846,7 @@
       </c>
       <c r="I502" s="2" t="inlineStr"/>
       <c r="J502" t="n">
-        <v>3.48</v>
+        <v>3.46</v>
       </c>
       <c r="K502" s="2" t="inlineStr"/>
       <c r="L502" s="2" t="inlineStr">
@@ -21896,7 +21888,7 @@
       </c>
       <c r="I503" s="2" t="inlineStr"/>
       <c r="J503" t="n">
-        <v>3.87</v>
+        <v>3.85</v>
       </c>
       <c r="K503" s="2" t="inlineStr"/>
       <c r="L503" s="2" t="inlineStr">
@@ -21938,7 +21930,7 @@
       </c>
       <c r="I504" s="2" t="inlineStr"/>
       <c r="J504" t="n">
-        <v>3.86</v>
+        <v>3.85</v>
       </c>
       <c r="K504" s="2" t="inlineStr"/>
       <c r="L504" s="2" t="inlineStr">
@@ -22022,7 +22014,7 @@
       </c>
       <c r="I506" s="2" t="inlineStr"/>
       <c r="J506" t="n">
-        <v>4.25</v>
+        <v>4.24</v>
       </c>
       <c r="K506" s="2" t="inlineStr"/>
       <c r="L506" s="2" t="inlineStr">
@@ -22846,7 +22838,7 @@
       </c>
       <c r="I526" s="2" t="inlineStr"/>
       <c r="J526" t="n">
-        <v>3.68</v>
+        <v>3.67</v>
       </c>
       <c r="K526" s="2" t="inlineStr"/>
       <c r="L526" s="2" t="inlineStr">
@@ -23266,7 +23258,7 @@
       </c>
       <c r="I536" s="2" t="inlineStr"/>
       <c r="J536" t="n">
-        <v>4.08</v>
+        <v>4.07</v>
       </c>
       <c r="K536" s="2" t="inlineStr"/>
       <c r="L536" s="2" t="inlineStr">
@@ -23938,7 +23930,7 @@
       </c>
       <c r="I552" s="2" t="inlineStr"/>
       <c r="J552" t="n">
-        <v>4.2</v>
+        <v>4.19</v>
       </c>
       <c r="K552" s="2" t="inlineStr"/>
       <c r="L552" s="2" t="inlineStr">
@@ -24568,7 +24560,7 @@
       </c>
       <c r="I567" s="2" t="inlineStr"/>
       <c r="J567" t="n">
-        <v>4.18</v>
+        <v>4.19</v>
       </c>
       <c r="K567" s="2" t="inlineStr"/>
       <c r="L567" s="2" t="inlineStr">

</xml_diff>